<commit_message>
update xml, upload documentation
</commit_message>
<xml_diff>
--- a/Arbeitszeitentabelle.xlsx
+++ b/Arbeitszeitentabelle.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin Kritzl\Schule\4AHITT\SEW\Java\Projekt_Threadee\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Basti\Documents\NEUER-DESKTOP\v\Schule\Eclipse\Roboterfabrik\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>Erceg</t>
   </si>
@@ -38,13 +38,22 @@
     <t>UML</t>
   </si>
   <si>
-    <t>Summe</t>
-  </si>
-  <si>
     <t>Requirement Analyse</t>
   </si>
   <si>
     <t>Egit</t>
+  </si>
+  <si>
+    <t>Summe/Person</t>
+  </si>
+  <si>
+    <t>Summe/Arbeitsschritt</t>
+  </si>
+  <si>
+    <t>Datum</t>
+  </si>
+  <si>
+    <t>Arbeitsschritt</t>
   </si>
 </sst>
 </file>
@@ -98,6 +107,24 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:F14" totalsRowShown="0">
+  <autoFilter ref="A1:F14"/>
+  <sortState ref="A2:F14">
+    <sortCondition ref="B1:B14"/>
+  </sortState>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Arbeitsschritt"/>
+    <tableColumn id="2" name="Datum"/>
+    <tableColumn id="3" name="Erceg"/>
+    <tableColumn id="4" name="Kritzl"/>
+    <tableColumn id="5" name="Steinkellner"/>
+    <tableColumn id="6" name="Summe/Arbeitsschritt"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -366,15 +393,24 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="3" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
@@ -385,7 +421,7 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -405,7 +441,7 @@
         <v>60</v>
       </c>
       <c r="F2">
-        <f>C2+D2+E2</f>
+        <f>SUM(C2:E2)</f>
         <v>180</v>
       </c>
     </row>
@@ -426,7 +462,7 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <f>C3+D3+E3</f>
+        <f>SUM(C3:E3)</f>
         <v>40</v>
       </c>
     </row>
@@ -447,50 +483,50 @@
         <v>70</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:F15" si="0">C4+D4+E4</f>
+        <f>SUM(C4:E4)</f>
         <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1">
         <v>41900</v>
       </c>
       <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
         <v>20</v>
       </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <f t="shared" si="0"/>
-        <v>23</v>
+        <f>SUM(C5:E5)</f>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1">
         <v>41900</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D6">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <f>SUM(C6:E6)</f>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -510,13 +546,13 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <f t="shared" si="0"/>
+        <f>SUM(C7:E7)</f>
         <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="1">
         <v>41903</v>
@@ -531,53 +567,72 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <f t="shared" si="0"/>
+        <f>SUM(C8:E8)</f>
         <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F9">
-        <f t="shared" si="0"/>
+        <f>SUM(C9:E9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F10">
-        <f t="shared" si="0"/>
+        <f>SUM(C10:E10)</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F11">
-        <f t="shared" si="0"/>
+        <f>SUM(C11:E11)</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F12">
-        <f t="shared" si="0"/>
+        <f>SUM(C12:E12)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F13">
-        <f t="shared" si="0"/>
+        <f>SUM(C13:E13)</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F14">
+        <f>SUM(C14:E14)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <f>SUM(C2:C14)</f>
+        <v>115</v>
+      </c>
+      <c r="D15">
+        <f t="shared" ref="D15:E15" si="0">SUM(D2:D14)</f>
+        <v>288</v>
+      </c>
+      <c r="E15">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
       <c r="F15">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>SUM(F2:F14)</f>
+        <v>533</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>